<commit_message>
Hien tien phat tung sach muon qua han
</commit_message>
<xml_diff>
--- a/PHIEUTHULIST.xlsx
+++ b/PHIEUTHULIST.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Danh sách phiếu thu</t>
   </si>
@@ -57,6 +57,24 @@
   </si>
   <si>
     <t>Giáo trình Hệ điều hành</t>
+  </si>
+  <si>
+    <t>PT010</t>
+  </si>
+  <si>
+    <t>Lê Thị Ngọc Ánh</t>
+  </si>
+  <si>
+    <t>Ngôn ngữ lập trình C#</t>
+  </si>
+  <si>
+    <t>PT011</t>
+  </si>
+  <si>
+    <t>Trần Lê Tuyết Mai</t>
+  </si>
+  <si>
+    <t>Đại số tuyến tính</t>
   </si>
 </sst>
 </file>
@@ -125,7 +143,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -224,6 +242,46 @@
         <v>8000</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3">
+        <v>46000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="3">
+        <v>33</v>
+      </c>
+      <c r="F8" s="3">
+        <v>66000</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:F1"/>

</xml_diff>

<commit_message>
Chỉnh giao diện code
</commit_message>
<xml_diff>
--- a/PHIEUTHULIST.xlsx
+++ b/PHIEUTHULIST.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Danh sách phiếu thu</t>
   </si>
@@ -33,6 +33,39 @@
   </si>
   <si>
     <t>Số tiền thu</t>
+  </si>
+  <si>
+    <t>PT002</t>
+  </si>
+  <si>
+    <t>Trần Nguyễn Yến Nhi</t>
+  </si>
+  <si>
+    <t>Cẩm nang chăm sóc sức khỏe</t>
+  </si>
+  <si>
+    <t>PT007</t>
+  </si>
+  <si>
+    <t>Toán học và ứng dụng</t>
+  </si>
+  <si>
+    <t>PT009</t>
+  </si>
+  <si>
+    <t>Nguyễn Thanh Hưng</t>
+  </si>
+  <si>
+    <t>Giáo trình Hệ điều hành</t>
+  </si>
+  <si>
+    <t>PT010</t>
+  </si>
+  <si>
+    <t>Lê Thị Ngọc Ánh</t>
+  </si>
+  <si>
+    <t>Ngôn ngữ lập trình C#</t>
   </si>
   <si>
     <t>PT011</t>
@@ -102,7 +135,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -110,8 +143,8 @@
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="12.2876968383789" customWidth="1"/>
-    <col min="3" max="3" width="16.4485026768276" customWidth="1"/>
-    <col min="4" max="4" width="15.5471823556083" customWidth="1"/>
+    <col min="3" max="3" width="19.1422337123326" customWidth="1"/>
+    <col min="4" max="4" width="26.443852015904" customWidth="1"/>
     <col min="5" max="5" width="12.9680350167411" customWidth="1"/>
     <col min="6" max="6" width="10.4410640171596" customWidth="1"/>
   </cols>
@@ -143,7 +176,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>7</v>
@@ -155,9 +188,89 @@
         <v>9</v>
       </c>
       <c r="E4" s="0">
+        <v>17</v>
+      </c>
+      <c r="F4" s="0">
+        <v>34000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>2</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="0">
+        <v>9</v>
+      </c>
+      <c r="F5" s="0">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="0">
+        <v>4</v>
+      </c>
+      <c r="F6" s="0">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>4</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="0">
+        <v>23</v>
+      </c>
+      <c r="F7" s="0">
+        <v>46000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>5</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="0">
         <v>33</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F8" s="0">
         <v>66000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hoan thien xuat Excel
</commit_message>
<xml_diff>
--- a/PHIEUTHULIST.xlsx
+++ b/PHIEUTHULIST.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Danh sách phiếu thu</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Đại số tuyến tính</t>
+  </si>
+  <si>
+    <t>PT012</t>
+  </si>
+  <si>
+    <t>Tổng tiền</t>
   </si>
 </sst>
 </file>
@@ -106,7 +112,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -114,16 +120,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="double"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" applyFont="1" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -135,19 +152,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.2876968383789" customWidth="1"/>
-    <col min="3" max="3" width="19.1422337123326" customWidth="1"/>
-    <col min="4" max="4" width="26.443852015904" customWidth="1"/>
-    <col min="5" max="5" width="12.9680350167411" customWidth="1"/>
-    <col min="6" max="6" width="10.4410640171596" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -274,9 +283,42 @@
         <v>66000</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>1002</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="0">
+        <v>43</v>
+      </c>
+      <c r="F9" s="0">
+        <v>86000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4">
+        <v>258000</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A10:E10"/>
   </mergeCells>
   <headerFooter/>
 </worksheet>

</xml_diff>